<commit_message>
Matlab file to process data
Matlab file to process data
</commit_message>
<xml_diff>
--- a/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/Comparison/Rat_Leg_Trials_ICs.xlsx
+++ b/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/Comparison/Rat_Leg_Trials_ICs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\Comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E4E615-9678-4831-BD53-78F124184369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC92F5F-576C-415B-B644-C3704790CC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3160410F-EDD1-440C-A3D7-26F242EE7A28}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3160410F-EDD1-440C-A3D7-26F242EE7A28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Muscle</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>resting</t>
+  </si>
+  <si>
+    <t>data doesn't match</t>
+  </si>
+  <si>
+    <t>missing 1 set</t>
   </si>
 </sst>
 </file>
@@ -99,12 +105,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,8 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F04492-FFE4-419F-88B8-D3107220F362}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,60 +486,66 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>93</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>143</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>155</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-18.55</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>54.6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>93</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>112</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>141</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -522,31 +555,38 @@
       <c r="C4">
         <v>113</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>88</v>
       </c>
       <c r="E4">
         <v>168</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>107</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>88</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -562,40 +602,52 @@
       <c r="E6">
         <v>141</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="J6" s="3">
+        <f>J5+J2</f>
+        <v>101.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>116</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>87</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>108</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>105</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>142</v>
       </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>